<commit_message>
Updated Excel file for card list
</commit_message>
<xml_diff>
--- a/cardshifter-database/TCG card list 10-27-14.xlsx
+++ b/cardshifter-database/TCG card list 10-27-14.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="25300" windowHeight="15380"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24800" windowHeight="15380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,9 +71,6 @@
     <t>Immolate</t>
   </si>
   <si>
-    <t xml:space="preserve">Poverty </t>
-  </si>
-  <si>
     <t xml:space="preserve">Rust Storm </t>
   </si>
   <si>
@@ -182,12 +179,6 @@
     <t>Head Shot</t>
   </si>
   <si>
-    <t>Destroy one Bio unit with 5 health or less.</t>
-  </si>
-  <si>
-    <t>Destroy one Bio unit with 6 health or more.</t>
-  </si>
-  <si>
     <t>Dumpster</t>
   </si>
   <si>
@@ -230,28 +221,37 @@
     <t>Opponent cannot play Bios next turn.</t>
   </si>
   <si>
-    <t>Owned Mechs gain 2 attack this turn only.</t>
-  </si>
-  <si>
-    <t>Upgrade a Bio unit 2/2 for a cost in Mana instead of Scrap.</t>
-  </si>
-  <si>
     <t>Firmware Upgrade</t>
   </si>
   <si>
     <t>Power Surge</t>
   </si>
   <si>
-    <t>Owned Mechs gain 2 durring next opponent turn.</t>
-  </si>
-  <si>
-    <t>Upgrade a Mech by 3/3 costing all of your Scrap.</t>
-  </si>
-  <si>
     <t>The next Upgrade you play this turn costs 0 Scrap.</t>
   </si>
   <si>
     <t>Opponent cannot play any Upgrade next turn.</t>
+  </si>
+  <si>
+    <t>Downgrade</t>
+  </si>
+  <si>
+    <t>Owned Mechs gain 2 Health during next opponent turn.</t>
+  </si>
+  <si>
+    <t>Owned Mechs gain 2 Attack this turn only.</t>
+  </si>
+  <si>
+    <t>Destroy one Bio unit with 5 Health or less.</t>
+  </si>
+  <si>
+    <t>Destroy one Bio unit with 6 Health or more.</t>
+  </si>
+  <si>
+    <t>Upgrade a Bio +2/+2 for a cost in Mana instead of Scrap.</t>
+  </si>
+  <si>
+    <t>Upgrade a Mech +3/+3 costing all of your Scrap.</t>
   </si>
 </sst>
 </file>
@@ -343,8 +343,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -384,9 +390,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -681,8 +693,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="700" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -692,17 +705,17 @@
     <col min="3" max="3" width="45" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.83203125" style="2"/>
     <col min="5" max="5" width="0" style="13" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="17"/>
+    <col min="6" max="6" width="5.83203125" style="17" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="0" style="17" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" style="17"/>
+    <col min="8" max="8" width="6" style="17" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="0" style="17" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="8.83203125" style="17"/>
+    <col min="10" max="10" width="9.5" style="17" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="0" style="17" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="8.83203125" style="17"/>
+    <col min="12" max="12" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="0" style="17" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="8.83203125" style="17"/>
     <col min="15" max="15" width="0" style="17" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="8.83203125" style="17"/>
+    <col min="16" max="16" width="7.33203125" style="17" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="0" style="17" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="8.83203125" style="17"/>
     <col min="19" max="16384" width="8.83203125" style="2"/>
@@ -766,7 +779,7 @@
     </row>
     <row r="2" spans="1:18">
       <c r="B2" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>11</v>
@@ -810,7 +823,7 @@
     </row>
     <row r="3" spans="1:18">
       <c r="B3" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
@@ -854,7 +867,7 @@
     </row>
     <row r="4" spans="1:18">
       <c r="B4" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>11</v>
@@ -898,7 +911,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="B5" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>11</v>
@@ -942,7 +955,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="B6" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
@@ -986,7 +999,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="B7" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>11</v>
@@ -1030,7 +1043,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="B8" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>11</v>
@@ -1074,7 +1087,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="B9" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>11</v>
@@ -1118,7 +1131,7 @@
     </row>
     <row r="10" spans="1:18">
       <c r="B10" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>11</v>
@@ -1162,7 +1175,7 @@
     </row>
     <row r="11" spans="1:18" s="3" customFormat="1">
       <c r="B11" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="3" t="s">
@@ -1209,7 +1222,7 @@
     </row>
     <row r="12" spans="1:18">
       <c r="B12" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>12</v>
@@ -1235,9 +1248,6 @@
       <c r="K12" s="4">
         <v>0</v>
       </c>
-      <c r="L12" s="17">
-        <v>0</v>
-      </c>
       <c r="O12" s="17">
         <v>1</v>
       </c>
@@ -1253,7 +1263,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="B13" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>12</v>
@@ -1279,9 +1289,6 @@
       <c r="K13" s="17">
         <v>0</v>
       </c>
-      <c r="L13" s="17">
-        <v>0</v>
-      </c>
       <c r="O13" s="17">
         <v>1</v>
       </c>
@@ -1297,7 +1304,7 @@
     </row>
     <row r="14" spans="1:18">
       <c r="B14" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>12</v>
@@ -1323,9 +1330,6 @@
       <c r="K14" s="17">
         <v>0</v>
       </c>
-      <c r="L14" s="17">
-        <v>0</v>
-      </c>
       <c r="O14" s="17">
         <v>1</v>
       </c>
@@ -1341,7 +1345,7 @@
     </row>
     <row r="15" spans="1:18">
       <c r="B15" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>12</v>
@@ -1367,9 +1371,6 @@
       <c r="K15" s="17">
         <v>0</v>
       </c>
-      <c r="L15" s="17">
-        <v>0</v>
-      </c>
       <c r="O15" s="17">
         <v>1</v>
       </c>
@@ -1385,7 +1386,7 @@
     </row>
     <row r="16" spans="1:18">
       <c r="B16" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>12</v>
@@ -1411,9 +1412,6 @@
       <c r="K16" s="17">
         <v>0</v>
       </c>
-      <c r="L16" s="17">
-        <v>0</v>
-      </c>
       <c r="O16" s="17">
         <v>1</v>
       </c>
@@ -1429,7 +1427,7 @@
     </row>
     <row r="17" spans="1:26">
       <c r="B17" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>12</v>
@@ -1455,9 +1453,6 @@
       <c r="K17" s="17">
         <v>0</v>
       </c>
-      <c r="L17" s="17">
-        <v>0</v>
-      </c>
       <c r="O17" s="17">
         <v>1</v>
       </c>
@@ -1473,7 +1468,7 @@
     </row>
     <row r="18" spans="1:26">
       <c r="B18" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>12</v>
@@ -1499,9 +1494,6 @@
       <c r="K18" s="17">
         <v>0</v>
       </c>
-      <c r="L18" s="17">
-        <v>0</v>
-      </c>
       <c r="O18" s="17">
         <v>1</v>
       </c>
@@ -1517,7 +1509,7 @@
     </row>
     <row r="19" spans="1:26" s="3" customFormat="1">
       <c r="B19" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="3" t="s">
@@ -1544,9 +1536,7 @@
       <c r="K19" s="19">
         <v>0</v>
       </c>
-      <c r="L19" s="19">
-        <v>0</v>
-      </c>
+      <c r="L19" s="19"/>
       <c r="M19" s="19"/>
       <c r="N19" s="19"/>
       <c r="O19" s="19">
@@ -1564,7 +1554,7 @@
     </row>
     <row r="20" spans="1:26">
       <c r="B20" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>13</v>
@@ -1590,7 +1580,7 @@
     </row>
     <row r="21" spans="1:26">
       <c r="B21" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>13</v>
@@ -1616,7 +1606,7 @@
     </row>
     <row r="22" spans="1:26">
       <c r="B22" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>13</v>
@@ -1642,7 +1632,7 @@
     </row>
     <row r="23" spans="1:26">
       <c r="B23" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>13</v>
@@ -1668,7 +1658,7 @@
     </row>
     <row r="24" spans="1:26">
       <c r="B24" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>13</v>
@@ -1694,7 +1684,7 @@
     </row>
     <row r="25" spans="1:26">
       <c r="B25" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>13</v>
@@ -1720,7 +1710,7 @@
     </row>
     <row r="26" spans="1:26">
       <c r="B26" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>13</v>
@@ -1746,7 +1736,7 @@
     </row>
     <row r="27" spans="1:26">
       <c r="B27" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>13</v>
@@ -1772,7 +1762,7 @@
     </row>
     <row r="28" spans="1:26">
       <c r="B28" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>13</v>
@@ -1799,13 +1789,13 @@
     <row r="29" spans="1:26">
       <c r="A29" s="5"/>
       <c r="B29" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E29" s="16"/>
       <c r="F29" s="21"/>
@@ -1835,13 +1825,13 @@
     <row r="30" spans="1:26">
       <c r="A30" s="11"/>
       <c r="B30" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E30" s="15"/>
       <c r="F30" s="4"/>
@@ -1870,13 +1860,13 @@
     </row>
     <row r="31" spans="1:26">
       <c r="B31" s="10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J31" s="17">
         <v>4</v>
@@ -1884,13 +1874,13 @@
     </row>
     <row r="32" spans="1:26">
       <c r="B32" s="10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J32" s="17">
         <v>4</v>
@@ -1898,13 +1888,13 @@
     </row>
     <row r="33" spans="2:10">
       <c r="B33" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J33" s="17">
         <v>6</v>
@@ -1912,13 +1902,13 @@
     </row>
     <row r="34" spans="2:10">
       <c r="B34" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J34" s="17">
         <v>4</v>
@@ -1929,24 +1919,24 @@
         <v>15</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J35" s="17">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="2:10">
       <c r="B36" s="10" t="s">
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J36" s="17">
         <v>7</v>
@@ -1954,13 +1944,13 @@
     </row>
     <row r="37" spans="2:10">
       <c r="B37" s="10" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J37" s="17">
         <v>3</v>
@@ -1968,13 +1958,22 @@
     </row>
     <row r="38" spans="2:10">
       <c r="B38" s="10" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="F38" s="17">
+        <v>2</v>
+      </c>
+      <c r="H38" s="17">
+        <v>2</v>
+      </c>
+      <c r="J38" s="17">
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="2:10">
@@ -1982,65 +1981,89 @@
         <v>17</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="F39" s="17">
+        <v>3</v>
+      </c>
+      <c r="H39" s="17">
+        <v>3</v>
+      </c>
+      <c r="J39" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="2:10">
       <c r="B40" s="10" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="J40" s="17">
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="2:10">
       <c r="B41" s="10" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="J41" s="17">
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="2:10">
       <c r="B42" s="10" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="J42" s="17">
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="2:10">
       <c r="B43" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="J43" s="17">
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="2:10">
       <c r="B44" s="10" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="J44" s="17">
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="2:10">
@@ -2048,10 +2071,13 @@
         <v>20</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="J45" s="17">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>